<commit_message>
Testing Table for Ordering Pizza Combos & Corresponding Selenium Tests
Although I’ve tested the browsers, I’m still going through the device
tests for the Testing Table—since there was a lot to do for the Table,
I figured I’d run with that and save time when going through the page
proper again later—so that document will probably be modified quite
frequently.
</commit_message>
<xml_diff>
--- a/Ordering Pizza Combinations, Jack Ferguson.xlsx
+++ b/Ordering Pizza Combinations, Jack Ferguson.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="14900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Deluxe</t>
   </si>
@@ -25,6 +30,159 @@
   </si>
   <si>
     <t>Cheese</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>No--can't remove pizza. Image off plum. Price wrong: £7.94 instead of £7.49</t>
+  </si>
+  <si>
+    <t>No--can't remove pizza. Image off plum. Says "Classic Deluxe" instead of "Classic Deluxe Pizza". Price fine.</t>
+  </si>
+  <si>
+    <t>No--can't remove pizza. Image off plum. Price fine.</t>
+  </si>
+  <si>
+    <t>No--can't remove pizza. Price fine.</t>
+  </si>
+  <si>
+    <t>No--can't remove either pizza. Intended price is wrong: should be 16.48, not 16.93</t>
+  </si>
+  <si>
+    <t>No--can remove neither pizza. Price wrong: should be £13.48</t>
+  </si>
+  <si>
+    <t>No--can't remove any pizza. Price should be £22.47, not 22.92</t>
+  </si>
+  <si>
+    <t>No--can't remove any pizza. Price fine.</t>
+  </si>
+  <si>
+    <t>No--can't remove any pizza. Price wrong: should be 25.47, not 25.92</t>
+  </si>
+  <si>
+    <t>Price fine; can't remove any pizza.</t>
+  </si>
+  <si>
+    <t>No--price should be 23.97 not 24.87.</t>
+  </si>
+  <si>
+    <t>No--can't remove pizzas; price should be 20.97, not 21.87</t>
+  </si>
+  <si>
+    <t>Price fine; can't remove pizzas, though.</t>
+  </si>
+  <si>
+    <t>No--can't remove pizzas; price should be 32.96, not 33.86</t>
+  </si>
+  <si>
+    <t>No--price should be 26.96, not 27.86; can't remove any pizza.</t>
+  </si>
+  <si>
+    <t>No--price should be 37.45, not 37.9; can't remove pizzas.</t>
+  </si>
+  <si>
+    <t>No--pizza should be 7.49, not 7.94</t>
+  </si>
+  <si>
+    <t>No--should be 16.48, not 16.93</t>
+  </si>
+  <si>
+    <t>No--should be 13.48, not 13.93</t>
+  </si>
+  <si>
+    <t>No--should be 22.47, not 22.92</t>
+  </si>
+  <si>
+    <t>No--should be 25.47, not 25.92</t>
+  </si>
+  <si>
+    <t>No--price should be 23.97, not 24.87</t>
+  </si>
+  <si>
+    <t>No--price should be 20.97, not 21.87</t>
+  </si>
+  <si>
+    <t>No--price should be 19.47, not 19.92</t>
+  </si>
+  <si>
+    <t>No--price should be 32.96, not 33.86</t>
+  </si>
+  <si>
+    <t>No--should be 26.96, not 27.86</t>
+  </si>
+  <si>
+    <t>No--price should be 37.45, not 37.9</t>
+  </si>
+  <si>
+    <t>No--price should be 38.95, not 39.85</t>
+  </si>
+  <si>
+    <t>No--price should be 35.95, not 36.85</t>
+  </si>
+  <si>
+    <t>No--price should be 44.94, not 45.84</t>
+  </si>
+  <si>
+    <t>No--price should be 7.49, not 7.94</t>
+  </si>
+  <si>
+    <t>No--price should be 38.95, not 39.85. Can't remove any pizza.</t>
+  </si>
+  <si>
+    <t>No--price should be 35.95, not 36.85. Can't remove any pizza.</t>
+  </si>
+  <si>
+    <t>No--price should be 44.94, not 45.84. Can't remove pizzas.</t>
+  </si>
+  <si>
+    <t>No--price should be 16.48, not 16.93.</t>
+  </si>
+  <si>
+    <t>No--can't remove pizzas; price should be 19.47, not 19.92</t>
+  </si>
+  <si>
+    <t>Kindle Fire</t>
+  </si>
+  <si>
+    <t>iPad4</t>
+  </si>
+  <si>
+    <t>iPhone 6</t>
+  </si>
+  <si>
+    <t>Nexus 10</t>
+  </si>
+  <si>
+    <t>Galaxy S4</t>
+  </si>
+  <si>
+    <t>Images off plum. Price fine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images off plum. Price fine. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No--pizza should be 7.49, not 7.94. Images off plum. </t>
+  </si>
+  <si>
+    <t>No--should be 16.48, not 16.93. Images off plum.</t>
+  </si>
+  <si>
+    <t>No--should be 13.48, not 13.93. Images off plum.</t>
+  </si>
+  <si>
+    <t>No--should be 25.47, not 25.92. Images off plum.</t>
   </si>
 </sst>
 </file>
@@ -366,20 +524,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="21" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="21" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -441,7 +609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -571,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -634,10 +802,271 @@
       </c>
       <c r="U4" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -647,9 +1076,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -659,8 +1093,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Ordering combo table across all devices and browsers.
More an artefact of the testing process than a major deliverable
inasmuch as its contents translate into test cases in the document
proper, but it’s there as evidence for use of various testing
techniques—and can be pointed to in a presentation.
</commit_message>
<xml_diff>
--- a/Ordering Pizza Combinations, Jack Ferguson.xlsx
+++ b/Ordering Pizza Combinations, Jack Ferguson.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="14900"/>
+    <workbookView xWindow="3860" yWindow="1180" windowWidth="22640" windowHeight="15180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="78">
   <si>
     <t>Deluxe</t>
   </si>
@@ -179,10 +179,82 @@
     <t>No--should be 16.48, not 16.93. Images off plum.</t>
   </si>
   <si>
-    <t>No--should be 13.48, not 13.93. Images off plum.</t>
-  </si>
-  <si>
     <t>No--should be 25.47, not 25.92. Images off plum.</t>
+  </si>
+  <si>
+    <t>No--price should be 7.49, not 7.94. Otherwise fine.</t>
+  </si>
+  <si>
+    <t>Price wrong. Otherwise fine.</t>
+  </si>
+  <si>
+    <t>Price wrong. Images off plum. Otherwise fine.</t>
+  </si>
+  <si>
+    <t>Fine.</t>
+  </si>
+  <si>
+    <t>Images offish. Otherwise fine.</t>
+  </si>
+  <si>
+    <t>Fine, though way zoomed out.</t>
+  </si>
+  <si>
+    <t>The two can definitely be added, but the price should be 16.48, not 16.93.</t>
+  </si>
+  <si>
+    <t>Price wrong. Fine, notwithstanding. (Maybe a juttery page?)</t>
+  </si>
+  <si>
+    <t>Price wrong, and images off plum; needs optimised because jutters. Can still add.</t>
+  </si>
+  <si>
+    <t>Price wrong but  can still add pizzas and remove. Fine, mostly.</t>
+  </si>
+  <si>
+    <t>Price wrong, but adds and removes pizzas fine.</t>
+  </si>
+  <si>
+    <t>Price wrong, but adds and removes pizzas fine. Zoomed out.</t>
+  </si>
+  <si>
+    <t>Price wrong, but adds and removes pizzas fine. Zoomed in.</t>
+  </si>
+  <si>
+    <t>No--should be 13.48, not 13.93. Images off plum. Fine for add</t>
+  </si>
+  <si>
+    <t>Price wrong, but adds and removes pizzas fine. Squashed.</t>
+  </si>
+  <si>
+    <t>Price wrong, but adds and removes pizzas fine. Squashed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price wrong, but adds and removes pizzas fine. </t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Yes. Squashed.</t>
+  </si>
+  <si>
+    <t>Yes. Zoomed out.</t>
+  </si>
+  <si>
+    <t>No, same price problem. Zoomed out.Adds and removes fine.</t>
+  </si>
+  <si>
+    <t>No, same price problem. Zoomed in. Adds and removes fine.</t>
+  </si>
+  <si>
+    <t>No, same price problem. Adds and removes fine.</t>
+  </si>
+  <si>
+    <t>Price wrong; adds and removes fine.</t>
+  </si>
+  <si>
+    <t>Wrong price; adds and removes fine.</t>
   </si>
 </sst>
 </file>
@@ -526,25 +598,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
-    <col min="11" max="11" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="21" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -1006,6 +1084,63 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>77</v>
+      </c>
+      <c r="R9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S9" t="s">
+        <v>77</v>
+      </c>
+      <c r="T9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
@@ -1014,6 +1149,63 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>77</v>
+      </c>
+      <c r="R10" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" t="s">
+        <v>77</v>
+      </c>
+      <c r="T10" t="s">
+        <v>77</v>
+      </c>
+      <c r="U10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
@@ -1022,6 +1214,63 @@
       <c r="B11" t="s">
         <v>48</v>
       </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R11" t="s">
+        <v>77</v>
+      </c>
+      <c r="S11" t="s">
+        <v>77</v>
+      </c>
+      <c r="T11" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
@@ -1030,6 +1279,63 @@
       <c r="B12" t="s">
         <v>3</v>
       </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>77</v>
+      </c>
+      <c r="R12" t="s">
+        <v>77</v>
+      </c>
+      <c r="S12" t="s">
+        <v>77</v>
+      </c>
+      <c r="T12" t="s">
+        <v>77</v>
+      </c>
+      <c r="U12" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
@@ -1044,20 +1350,56 @@
       <c r="D13" t="s">
         <v>50</v>
       </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
       <c r="F13" t="s">
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
         <v>48</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" t="s">
+        <v>77</v>
+      </c>
+      <c r="S13" t="s">
+        <v>77</v>
+      </c>
+      <c r="T13" t="s">
+        <v>77</v>
+      </c>
+      <c r="U13" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>